<commit_message>
Update to Criminal History 4.1 migration
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Query_Results_Service/artifacts/service_model/information_model/Criminal_History-IEPD/documentation/Rapsheet_4.0To4.1.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Query_Results_Service/artifacts/service_model/information_model/Criminal_History-IEPD/documentation/Rapsheet_4.0To4.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="10365"/>
+    <workbookView xWindow="1560" yWindow="465" windowWidth="24660" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>Crimianl History / Rapsheet 4.0 / NIEM 2.0 Mapping</t>
   </si>
   <si>
-    <t>/ch-doc:CriminalHistory/rap:RapSheet/rap:RapSheetCycle/rap:Arrest/rap:ArrestCharge</t>
-  </si>
-  <si>
     <t>/ch-doc:CriminalHistory/ch:RapSheet/ch:RapSheetPerson/jxdm:PersonAugmentation/jxdm:PersonStateFingerprintIdentification/nc:IdentificationSourceText</t>
   </si>
   <si>
@@ -83,18 +80,6 @@
   </si>
   <si>
     <t>Sentence Description Text</t>
-  </si>
-  <si>
-    <t>/ch-doc:CriminalHistory/rap:RapSheet/rap:RapSheetCycle/rap:Prosecution/rap:ProsecutionCharge</t>
-  </si>
-  <si>
-    <t>/ch-doc:CriminalHistory/rap:RapSheet/rap:RapSheetCycle/rap:Prosecution/rap:ProsecutionCharge/rap:ChargeStatute</t>
-  </si>
-  <si>
-    <t>/ch-doc:CriminalHistory/rap:RapSheet/rap:RapSheetCycle/rap:CourtAction/nc:ActivityIdentification/nc:IdentificationJurisdictionText</t>
-  </si>
-  <si>
-    <t>/ch-doc:CriminalHistory/rap:RapSheet/rap:RapSheetCycle/rap:CourtAction/rap:CourtCharge</t>
   </si>
   <si>
     <t>/ch-doc:CriminalHistory/ch-ext:RapSheet/ch-ext:Person</t>
@@ -200,6 +185,21 @@
 xmlns:j=http://niem.gov/niem/domains/jxdm/4.0 to
 xmlns:j="http://niem.gov/niem/domains/jxdm/4.1"</t>
     </r>
+  </si>
+  <si>
+    <t>/ch-doc:CriminalHistory/ch-ext:RapSheet/ch-ext:RapSheetCycle/rap:Arrest/rap:ArrestCharge</t>
+  </si>
+  <si>
+    <t>/ch-doc:CriminalHistory/ch-ext:RapSheet/ch-ext:RapSheetCycle/rap:Prosecution/rap:ProsecutionCharge</t>
+  </si>
+  <si>
+    <t>/ch-doc:CriminalHistory/rap:RapSheet/ch-ext:RapSheetCycle/rap:Prosecution/rap:ProsecutionCharge/rap:ChargeStatute</t>
+  </si>
+  <si>
+    <t>/ch-doc:CriminalHistory/ch-ext:RapSheet/ch-ext:RapSheetCycle/rap:CourtAction/nc:ActivityIdentification/nc:IdentificationJurisdictionText</t>
+  </si>
+  <si>
+    <t>/ch-doc:CriminalHistory/ch-ext:RapSheet/ch-ext:RapSheetCycle/rap:CourtAction/rap:CourtCharge</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1224,10 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,10 +1270,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -1281,14 +1281,14 @@
     </row>
     <row r="4" spans="1:8" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="16"/>
@@ -1297,14 +1297,14 @@
     </row>
     <row r="5" spans="1:8" s="11" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="16"/>
@@ -1313,14 +1313,14 @@
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="10"/>
@@ -1329,14 +1329,14 @@
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="10"/>
@@ -1345,14 +1345,14 @@
     </row>
     <row r="8" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="10"/>
@@ -1361,13 +1361,13 @@
     </row>
     <row r="9" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1375,14 +1375,14 @@
     </row>
     <row r="10" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="10"/>
@@ -1391,14 +1391,14 @@
     </row>
     <row r="11" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="10"/>
@@ -1407,14 +1407,14 @@
     </row>
     <row r="12" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="10"/>
@@ -1423,14 +1423,14 @@
     </row>
     <row r="13" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="10"/>
@@ -1439,14 +1439,14 @@
     </row>
     <row r="14" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="10"/>
@@ -1455,14 +1455,14 @@
     </row>
     <row r="15" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="10"/>
@@ -1471,14 +1471,14 @@
     </row>
     <row r="16" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -1487,14 +1487,14 @@
     </row>
     <row r="17" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="10"/>
@@ -1503,12 +1503,12 @@
     </row>
     <row r="18" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="10"/>
@@ -1517,12 +1517,12 @@
     </row>
     <row r="19" spans="1:8" s="7" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="10"/>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="20" spans="1:8" s="7" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="10"/>

</xml_diff>